<commit_message>
Updated Data Access from Excel sheet for MSO Tests
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\git\AutomationWrapper\LiberateAutomation\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95214283-7F09-4E57-8155-0D917000D464}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -40,12 +46,60 @@
   </si>
   <si>
     <t>ANSQ</t>
+  </si>
+  <si>
+    <t>SOEnquire</t>
+  </si>
+  <si>
+    <t>A00071A</t>
+  </si>
+  <si>
+    <t>RouteSO</t>
+  </si>
+  <si>
+    <t>RedirectSO</t>
+  </si>
+  <si>
+    <t>BrowseSO</t>
+  </si>
+  <si>
+    <t>AssignSO</t>
+  </si>
+  <si>
+    <t>ZA00103</t>
+  </si>
+  <si>
+    <t>SplitSO</t>
+  </si>
+  <si>
+    <t>WI00204</t>
+  </si>
+  <si>
+    <t>YE00194</t>
+  </si>
+  <si>
+    <t>SuspendSO</t>
+  </si>
+  <si>
+    <t>ManualWaitlistSO</t>
+  </si>
+  <si>
+    <t>WaitlistSO</t>
+  </si>
+  <si>
+    <t>RejectSO</t>
+  </si>
+  <si>
+    <t>AccountSO</t>
+  </si>
+  <si>
+    <t>GeneralSO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,11 +135,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{489728C4-8CAF-458C-AAA4-F28F3EEFDC0E}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -134,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,9 +252,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,6 +304,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -377,11 +496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,13 +540,85 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -439,7 +630,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Completed Provide Set Top Box Test Case
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15600" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="4890"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -91,12 +92,24 @@
   </si>
   <si>
     <t>alterSIMService</t>
+  </si>
+  <si>
+    <t>setTopBoxService</t>
+  </si>
+  <si>
+    <t>928104</t>
+  </si>
+  <si>
+    <t>setTopBoxProduct</t>
+  </si>
+  <si>
+    <t>50010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,9 +263,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +315,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="A18:B18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +630,22 @@
       </c>
       <c r="B17" s="1">
         <v>9291476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Test cases for Cease multiple services and Count of service products
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>9281508</t>
+  </si>
+  <si>
+    <t>ceasemultipleserviceaccount</t>
+  </si>
+  <si>
+    <t>280002720000</t>
+  </si>
+  <si>
+    <t>CountofServiceProducts</t>
+  </si>
+  <si>
+    <t>9177989</t>
   </si>
 </sst>
 </file>
@@ -484,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -630,6 +642,22 @@
       </c>
       <c r="B20" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exchange Signoff and LImeLite Issue fixed
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>1876071</t>
+  </si>
+  <si>
+    <t>exchangesignoffserviceordernumber</t>
+  </si>
+  <si>
+    <t>ZH00756</t>
+  </si>
+  <si>
+    <t>PEL_PDL_LimeLitePackage</t>
+  </si>
+  <si>
+    <t>Auto_PEL-PEL_WithoutRoutes (PEL)</t>
   </si>
 </sst>
 </file>
@@ -526,15 +538,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -728,6 +740,22 @@
       </c>
       <c r="B27" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing Query Management cases and Existing customer provisioning
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nphanide\git\AutomationWrapper\LiberateAutomation\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmallu\git\AutomationWrapper\AutomationWrapper\AutomationWrapper\LiberateAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -168,13 +168,38 @@
   </si>
   <si>
     <t>Auto_PEL-PEL_WithoutRoutes (PEL)</t>
+  </si>
+  <si>
+    <t>queryAccountNumber</t>
+  </si>
+  <si>
+    <t>260002260000</t>
+  </si>
+  <si>
+    <t>B00027E</t>
+  </si>
+  <si>
+    <t>nonAccountQuery</t>
+  </si>
+  <si>
+    <t>manageQueryNumber</t>
+  </si>
+  <si>
+    <t>B00028E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,6 +353,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -362,6 +405,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -538,224 +598,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>9291476</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing Existing customerPDL test case
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>B00028E</t>
+  </si>
+  <si>
+    <t>PDLServicePackage</t>
+  </si>
+  <si>
+    <t>ADSL Test</t>
   </si>
 </sst>
 </file>
@@ -598,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,6 +847,14 @@
       </c>
       <c r="B32" s="2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed screenshot issues for CloneServiceTC -Fixed cloneAccount -Fixed createSubAccount-Fixed
PaymentEnquiries- Account number

TransferProductTC -Fixed
POSPaymentTC: -Fixed
CeaseMultipleServicesTC -Done
alterlineproduct:-Done
</commit_message>
<xml_diff>
--- a/LiberateAutomation/Resources/DataSheet.xlsx
+++ b/LiberateAutomation/Resources/DataSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmallu\git\AutomationWrapper\AutomationWrapper\AutomationWrapper\LiberateAutomation\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nphanide\git\AutomationWrapper\LiberateAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>SalesDepartment</t>
   </si>
@@ -300,12 +300,15 @@
   </si>
   <si>
     <t>Sanity_Site</t>
+  </si>
+  <si>
+    <t>280007070000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -367,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -384,6 +387,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -508,23 +515,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -560,23 +550,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -753,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,6 +1178,14 @@
       </c>
       <c r="B55" s="7" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>